<commit_message>
further changes and added files
</commit_message>
<xml_diff>
--- a/real_data.xlsx
+++ b/real_data.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\PycharmProjects\Shelter-Routing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D61B111-F330-4814-87C9-B20BB7D5DE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8582D32-AAB0-40C0-8E95-10C6F57CF314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1778" yWindow="1778" windowWidth="15390" windowHeight="9442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Params" sheetId="1" r:id="rId1"/>
     <sheet name="Demand" sheetId="2" r:id="rId2"/>
     <sheet name="Distance" sheetId="4" r:id="rId3"/>
+    <sheet name="Coordinates" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>param</t>
   </si>
@@ -63,12 +64,18 @@
   <si>
     <t>demand</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +88,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,14 +130,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,13 +443,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+    <sheetView zoomScale="139" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -449,7 +465,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -457,7 +473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -465,7 +481,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -473,7 +489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -494,9 +510,9 @@
       <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -504,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -512,7 +528,7 @@
         <v>11548</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -520,7 +536,7 @@
         <v>14500</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -528,7 +544,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -536,7 +552,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -544,7 +560,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -552,7 +568,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -560,7 +576,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -568,7 +584,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -576,7 +592,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -584,7 +600,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -592,7 +608,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -600,7 +616,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -608,7 +624,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -616,7 +632,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -624,7 +640,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -632,7 +648,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -640,7 +656,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -648,7 +664,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -656,7 +672,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -664,7 +680,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -672,7 +688,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -680,7 +696,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -688,7 +704,7 @@
         <v>27022</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -696,7 +712,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -704,7 +720,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -712,7 +728,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -720,7 +736,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -728,7 +744,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -736,7 +752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -744,7 +760,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -752,7 +768,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -760,7 +776,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -768,7 +784,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -776,7 +792,7 @@
         <v>3073</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -784,7 +800,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -792,7 +808,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -800,7 +816,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -808,7 +824,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -816,7 +832,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -824,7 +840,7 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -832,7 +848,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -840,7 +856,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -848,7 +864,7 @@
         <v>11538</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -856,7 +872,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -864,7 +880,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -872,7 +888,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -880,7 +896,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -888,7 +904,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -896,7 +912,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -904,7 +920,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -912,7 +928,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -920,7 +936,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -928,7 +944,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -936,7 +952,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -944,7 +960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -952,7 +968,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -960,7 +976,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -968,7 +984,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -976,7 +992,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -984,7 +1000,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -992,7 +1008,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -1000,7 +1016,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1008,7 +1024,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -1016,7 +1032,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -1024,7 +1040,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -1032,7 +1048,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -1040,7 +1056,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -1048,7 +1064,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -1056,7 +1072,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -1064,7 +1080,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -1072,7 +1088,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -1088,7 +1104,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -1096,7 +1112,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -1104,7 +1120,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -1112,7 +1128,7 @@
         <v>2093</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -1120,7 +1136,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -1128,7 +1144,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -1136,7 +1152,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -1144,7 +1160,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -1152,7 +1168,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -1160,7 +1176,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -1168,7 +1184,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -1176,7 +1192,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -1184,7 +1200,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -1192,7 +1208,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -1200,7 +1216,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -1208,7 +1224,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -1216,7 +1232,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -1224,7 +1240,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -1232,7 +1248,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -1240,7 +1256,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -1248,7 +1264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -1256,7 +1272,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -1264,7 +1280,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -1272,7 +1288,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -1280,7 +1296,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -1288,7 +1304,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -1296,7 +1312,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -1304,7 +1320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -1312,7 +1328,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -1320,7 +1336,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -1328,7 +1344,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -1336,7 +1352,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -1344,7 +1360,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -1352,7 +1368,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -1360,7 +1376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -1368,7 +1384,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -1376,7 +1392,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -1384,7 +1400,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -1392,7 +1408,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -1400,7 +1416,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -1408,7 +1424,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -1416,7 +1432,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -1424,7 +1440,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -1432,7 +1448,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -1440,7 +1456,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -1448,7 +1464,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -1456,7 +1472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -1464,7 +1480,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -1472,7 +1488,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -1480,7 +1496,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -1488,7 +1504,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -1496,7 +1512,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -1504,7 +1520,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -1512,7 +1528,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -1520,7 +1536,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -1528,7 +1544,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -1536,7 +1552,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -1544,7 +1560,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -1552,7 +1568,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -1560,7 +1576,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -1568,7 +1584,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -1576,7 +1592,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -1584,7 +1600,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -1592,7 +1608,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -1600,7 +1616,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -1608,7 +1624,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -1616,7 +1632,7 @@
         <v>3061</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -1624,7 +1640,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -1632,7 +1648,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -1640,7 +1656,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -1648,7 +1664,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -1656,7 +1672,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -1664,7 +1680,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -1672,7 +1688,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -1680,7 +1696,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -1688,7 +1704,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -1696,7 +1712,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -1717,9 +1733,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:151" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>0</v>
       </c>
@@ -2171,7 +2187,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2626,7 +2642,7 @@
         <v>0.6208402275686733</v>
       </c>
     </row>
-    <row r="3" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3081,7 +3097,7 @@
         <v>0.48970955301080038</v>
       </c>
     </row>
-    <row r="4" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3536,7 +3552,7 @@
         <v>0.3379484264501047</v>
       </c>
     </row>
-    <row r="5" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3991,7 +4007,7 @@
         <v>0.36604725821630352</v>
       </c>
     </row>
-    <row r="6" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4446,7 +4462,7 @@
         <v>0.33663048327839079</v>
       </c>
     </row>
-    <row r="7" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4901,7 +4917,7 @@
         <v>0.37968710001208161</v>
       </c>
     </row>
-    <row r="8" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5356,7 +5372,7 @@
         <v>0.25075518460510898</v>
       </c>
     </row>
-    <row r="9" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5811,7 +5827,7 @@
         <v>0.3976459152700399</v>
       </c>
     </row>
-    <row r="10" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -6266,7 +6282,7 @@
         <v>0.33063489340786439</v>
       </c>
     </row>
-    <row r="11" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -6721,7 +6737,7 @@
         <v>0.5383589769894167</v>
       </c>
     </row>
-    <row r="12" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7176,7 +7192,7 @@
         <v>0.5243113129456729</v>
       </c>
     </row>
-    <row r="13" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7631,7 +7647,7 @@
         <v>0.32909241946333012</v>
       </c>
     </row>
-    <row r="14" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8086,7 +8102,7 @@
         <v>0.32769743176087007</v>
       </c>
     </row>
-    <row r="15" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8541,7 +8557,7 @@
         <v>0.29799464204029352</v>
       </c>
     </row>
-    <row r="16" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8996,7 +9012,7 @@
         <v>0.33610916633997773</v>
       </c>
     </row>
-    <row r="17" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -9451,7 +9467,7 @@
         <v>0.46162994021599379</v>
       </c>
     </row>
-    <row r="18" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -9906,7 +9922,7 @@
         <v>0.42590659240147871</v>
       </c>
     </row>
-    <row r="19" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -10361,7 +10377,7 @@
         <v>0.49752936408392562</v>
       </c>
     </row>
-    <row r="20" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -10816,7 +10832,7 @@
         <v>0.58255412746155621</v>
       </c>
     </row>
-    <row r="21" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -11271,7 +11287,7 @@
         <v>0.73075223367445252</v>
       </c>
     </row>
-    <row r="22" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -11726,7 +11742,7 @@
         <v>0.55938149098635592</v>
       </c>
     </row>
-    <row r="23" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -12181,7 +12197,7 @@
         <v>0.55938149098635592</v>
       </c>
     </row>
-    <row r="24" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -12636,7 +12652,7 @@
         <v>0.86781612403051522</v>
       </c>
     </row>
-    <row r="25" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -13091,7 +13107,7 @@
         <v>0.62508303879779226</v>
       </c>
     </row>
-    <row r="26" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -13546,7 +13562,7 @@
         <v>0.58650143926623299</v>
       </c>
     </row>
-    <row r="27" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -14001,7 +14017,7 @@
         <v>0.59014600946021989</v>
       </c>
     </row>
-    <row r="28" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -14456,7 +14472,7 @@
         <v>0.65264003150324168</v>
       </c>
     </row>
-    <row r="29" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -14911,7 +14927,7 @@
         <v>0.53010731141237422</v>
       </c>
     </row>
-    <row r="30" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -15366,7 +15382,7 @@
         <v>0.6509591116696688</v>
       </c>
     </row>
-    <row r="31" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -15821,7 +15837,7 @@
         <v>0.58234245700637244</v>
       </c>
     </row>
-    <row r="32" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -16276,7 +16292,7 @@
         <v>0.72326668977899389</v>
       </c>
     </row>
-    <row r="33" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -16731,7 +16747,7 @@
         <v>0.63009864627421341</v>
       </c>
     </row>
-    <row r="34" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -17186,7 +17202,7 @@
         <v>0.61685213438564956</v>
       </c>
     </row>
-    <row r="35" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -17641,7 +17657,7 @@
         <v>1.0143178982204011</v>
       </c>
     </row>
-    <row r="36" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -18096,7 +18112,7 @@
         <v>0.57112687580291954</v>
       </c>
     </row>
-    <row r="37" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -18551,7 +18567,7 @@
         <v>0.50169234890845282</v>
       </c>
     </row>
-    <row r="38" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -19006,7 +19022,7 @@
         <v>0.96609135923602629</v>
       </c>
     </row>
-    <row r="39" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -19461,7 +19477,7 @@
         <v>0.69768197928461029</v>
       </c>
     </row>
-    <row r="40" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -19916,7 +19932,7 @@
         <v>0.70390495288805177</v>
       </c>
     </row>
-    <row r="41" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -20371,7 +20387,7 @@
         <v>0.8250117777383863</v>
       </c>
     </row>
-    <row r="42" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -20826,7 +20842,7 @@
         <v>0.56727550852970809</v>
       </c>
     </row>
-    <row r="43" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -21281,7 +21297,7 @@
         <v>0.42310226477163998</v>
       </c>
     </row>
-    <row r="44" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -21736,7 +21752,7 @@
         <v>0.55634266469181815</v>
       </c>
     </row>
-    <row r="45" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -22191,7 +22207,7 @@
         <v>0.39737124552151232</v>
       </c>
     </row>
-    <row r="46" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -22646,7 +22662,7 @@
         <v>0.39974025408552288</v>
       </c>
     </row>
-    <row r="47" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -23101,7 +23117,7 @@
         <v>0.40586026460988989</v>
       </c>
     </row>
-    <row r="48" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -23556,7 +23572,7 @@
         <v>0.4396927457941589</v>
       </c>
     </row>
-    <row r="49" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -24011,7 +24027,7 @@
         <v>0.46716715756281357</v>
       </c>
     </row>
-    <row r="50" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -24466,7 +24482,7 @@
         <v>0.46109688703255253</v>
       </c>
     </row>
-    <row r="51" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -24921,7 +24937,7 @@
         <v>0.73758178377226191</v>
       </c>
     </row>
-    <row r="52" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -25376,7 +25392,7 @@
         <v>0.36598615500298087</v>
       </c>
     </row>
-    <row r="53" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -25831,7 +25847,7 @@
         <v>0.36785024837322478</v>
       </c>
     </row>
-    <row r="54" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -26286,7 +26302,7 @@
         <v>0.28648555883328197</v>
       </c>
     </row>
-    <row r="55" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -26741,7 +26757,7 @@
         <v>0.33805378031798528</v>
       </c>
     </row>
-    <row r="56" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -27196,7 +27212,7 @@
         <v>0.33058227124368877</v>
       </c>
     </row>
-    <row r="57" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -27651,7 +27667,7 @@
         <v>0.35795343470422158</v>
       </c>
     </row>
-    <row r="58" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
@@ -28106,7 +28122,7 @@
         <v>0.37800277098569518</v>
       </c>
     </row>
-    <row r="59" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
@@ -28561,7 +28577,7 @@
         <v>0.37923878094175739</v>
       </c>
     </row>
-    <row r="60" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
@@ -29016,7 +29032,7 @@
         <v>0.33495744882125911</v>
       </c>
     </row>
-    <row r="61" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>59</v>
       </c>
@@ -29471,7 +29487,7 @@
         <v>0.30273914441852162</v>
       </c>
     </row>
-    <row r="62" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>60</v>
       </c>
@@ -29926,7 +29942,7 @@
         <v>0.31872076179469999</v>
       </c>
     </row>
-    <row r="63" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>61</v>
       </c>
@@ -30381,7 +30397,7 @@
         <v>0.33519329853757879</v>
       </c>
     </row>
-    <row r="64" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>62</v>
       </c>
@@ -30836,7 +30852,7 @@
         <v>0.31145217636422962</v>
       </c>
     </row>
-    <row r="65" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>63</v>
       </c>
@@ -31291,7 +31307,7 @@
         <v>0.27568376896209179</v>
       </c>
     </row>
-    <row r="66" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>64</v>
       </c>
@@ -31746,7 +31762,7 @@
         <v>0.27129041935395742</v>
       </c>
     </row>
-    <row r="67" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>65</v>
       </c>
@@ -32201,7 +32217,7 @@
         <v>0.27129041935395742</v>
       </c>
     </row>
-    <row r="68" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>66</v>
       </c>
@@ -32656,7 +32672,7 @@
         <v>0.22323886489903391</v>
       </c>
     </row>
-    <row r="69" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>67</v>
       </c>
@@ -33111,7 +33127,7 @@
         <v>0.25972822007582191</v>
       </c>
     </row>
-    <row r="70" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>68</v>
       </c>
@@ -33566,7 +33582,7 @@
         <v>0.21391610968636779</v>
       </c>
     </row>
-    <row r="71" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>69</v>
       </c>
@@ -34021,7 +34037,7 @@
         <v>0.30284385555537258</v>
       </c>
     </row>
-    <row r="72" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>70</v>
       </c>
@@ -34476,7 +34492,7 @@
         <v>0.2278333964421056</v>
       </c>
     </row>
-    <row r="73" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
@@ -34931,7 +34947,7 @@
         <v>0.26909410085462848</v>
       </c>
     </row>
-    <row r="74" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
@@ -35386,7 +35402,7 @@
         <v>0.3015662952449169</v>
       </c>
     </row>
-    <row r="75" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>73</v>
       </c>
@@ -35841,7 +35857,7 @@
         <v>0.22465147086367571</v>
       </c>
     </row>
-    <row r="76" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>74</v>
       </c>
@@ -36296,7 +36312,7 @@
         <v>0.2187899800164487</v>
       </c>
     </row>
-    <row r="77" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
@@ -36751,7 +36767,7 @@
         <v>0.25163418759979511</v>
       </c>
     </row>
-    <row r="78" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
@@ -37206,7 +37222,7 @@
         <v>0.25163418759979511</v>
       </c>
     </row>
-    <row r="79" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>77</v>
       </c>
@@ -37661,7 +37677,7 @@
         <v>0.30087420841737222</v>
       </c>
     </row>
-    <row r="80" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>78</v>
       </c>
@@ -38116,7 +38132,7 @@
         <v>0.23012551901357331</v>
       </c>
     </row>
-    <row r="81" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>79</v>
       </c>
@@ -38571,7 +38587,7 @@
         <v>0.26574174080457369</v>
       </c>
     </row>
-    <row r="82" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>80</v>
       </c>
@@ -39026,7 +39042,7 @@
         <v>0.2294738119476786</v>
       </c>
     </row>
-    <row r="83" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
@@ -39481,7 +39497,7 @@
         <v>0.2789209372912525</v>
       </c>
     </row>
-    <row r="84" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>82</v>
       </c>
@@ -39936,7 +39952,7 @@
         <v>0.33129037661071142</v>
       </c>
     </row>
-    <row r="85" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>83</v>
       </c>
@@ -40391,7 +40407,7 @@
         <v>0.31350296563181201</v>
       </c>
     </row>
-    <row r="86" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>84</v>
       </c>
@@ -40846,7 +40862,7 @@
         <v>0.3146279311207299</v>
       </c>
     </row>
-    <row r="87" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>85</v>
       </c>
@@ -41301,7 +41317,7 @@
         <v>0.19366101323691001</v>
       </c>
     </row>
-    <row r="88" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>86</v>
       </c>
@@ -41756,7 +41772,7 @@
         <v>0.35108195085557309</v>
       </c>
     </row>
-    <row r="89" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>87</v>
       </c>
@@ -42211,7 +42227,7 @@
         <v>0.36194056170430489</v>
       </c>
     </row>
-    <row r="90" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>88</v>
       </c>
@@ -42666,7 +42682,7 @@
         <v>0.20039459953028721</v>
       </c>
     </row>
-    <row r="91" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>89</v>
       </c>
@@ -43121,7 +43137,7 @@
         <v>0.34242020777541932</v>
       </c>
     </row>
-    <row r="92" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>90</v>
       </c>
@@ -43576,7 +43592,7 @@
         <v>0.35533726871118693</v>
       </c>
     </row>
-    <row r="93" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>91</v>
       </c>
@@ -44031,7 +44047,7 @@
         <v>0.3097149025897164</v>
       </c>
     </row>
-    <row r="94" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>92</v>
       </c>
@@ -44486,7 +44502,7 @@
         <v>0.18358411469985761</v>
       </c>
     </row>
-    <row r="95" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>93</v>
       </c>
@@ -44941,7 +44957,7 @@
         <v>0.13933732964653189</v>
       </c>
     </row>
-    <row r="96" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>94</v>
       </c>
@@ -45396,7 +45412,7 @@
         <v>8.5054685645547953E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>95</v>
       </c>
@@ -45851,7 +45867,7 @@
         <v>0.20690765804210889</v>
       </c>
     </row>
-    <row r="98" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>96</v>
       </c>
@@ -46306,7 +46322,7 @@
         <v>8.400231890278681E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>97</v>
       </c>
@@ -46761,7 +46777,7 @@
         <v>0.1516106231786771</v>
       </c>
     </row>
-    <row r="100" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>98</v>
       </c>
@@ -47216,7 +47232,7 @@
         <v>0.21679525222156751</v>
       </c>
     </row>
-    <row r="101" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>99</v>
       </c>
@@ -47671,7 +47687,7 @@
         <v>0.17644829665837519</v>
       </c>
     </row>
-    <row r="102" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>100</v>
       </c>
@@ -48126,7 +48142,7 @@
         <v>0.16236907377208659</v>
       </c>
     </row>
-    <row r="103" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>101</v>
       </c>
@@ -48581,7 +48597,7 @@
         <v>0.20336728343067531</v>
       </c>
     </row>
-    <row r="104" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>102</v>
       </c>
@@ -49036,7 +49052,7 @@
         <v>0.13331122830439929</v>
       </c>
     </row>
-    <row r="105" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>103</v>
       </c>
@@ -49491,7 +49507,7 @@
         <v>0.20722508762364389</v>
       </c>
     </row>
-    <row r="106" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>104</v>
       </c>
@@ -49946,7 +49962,7 @@
         <v>0.18640278286635131</v>
       </c>
     </row>
-    <row r="107" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>105</v>
       </c>
@@ -50401,7 +50417,7 @@
         <v>0.20986985024868421</v>
       </c>
     </row>
-    <row r="108" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>106</v>
       </c>
@@ -50856,7 +50872,7 @@
         <v>0.20429747502453591</v>
       </c>
     </row>
-    <row r="109" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>107</v>
       </c>
@@ -51311,7 +51327,7 @@
         <v>0.15242818987455539</v>
       </c>
     </row>
-    <row r="110" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>108</v>
       </c>
@@ -51766,7 +51782,7 @@
         <v>0.13509524858691199</v>
       </c>
     </row>
-    <row r="111" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>109</v>
       </c>
@@ -52221,7 +52237,7 @@
         <v>0.2031773317790507</v>
       </c>
     </row>
-    <row r="112" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>110</v>
       </c>
@@ -52676,7 +52692,7 @@
         <v>0.1466387574497863</v>
       </c>
     </row>
-    <row r="113" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>111</v>
       </c>
@@ -53131,7 +53147,7 @@
         <v>0.21519195161613541</v>
       </c>
     </row>
-    <row r="114" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>112</v>
       </c>
@@ -53586,7 +53602,7 @@
         <v>0.21474463843018821</v>
       </c>
     </row>
-    <row r="115" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>113</v>
       </c>
@@ -54041,7 +54057,7 @@
         <v>0.16816530291444401</v>
       </c>
     </row>
-    <row r="116" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>114</v>
       </c>
@@ -54496,7 +54512,7 @@
         <v>0.10994559641788169</v>
       </c>
     </row>
-    <row r="117" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>115</v>
       </c>
@@ -54951,7 +54967,7 @@
         <v>7.2042042468682177E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>116</v>
       </c>
@@ -55406,7 +55422,7 @@
         <v>0.1434765893312254</v>
       </c>
     </row>
-    <row r="119" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>117</v>
       </c>
@@ -55861,7 +55877,7 @@
         <v>0.15654652717304371</v>
       </c>
     </row>
-    <row r="120" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>118</v>
       </c>
@@ -56316,7 +56332,7 @@
         <v>0.14374534848357801</v>
       </c>
     </row>
-    <row r="121" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>119</v>
       </c>
@@ -56771,7 +56787,7 @@
         <v>0.13717814337663109</v>
       </c>
     </row>
-    <row r="122" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>120</v>
       </c>
@@ -57226,7 +57242,7 @@
         <v>0.18081405815549731</v>
       </c>
     </row>
-    <row r="123" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>121</v>
       </c>
@@ -57681,7 +57697,7 @@
         <v>0.14780329250369481</v>
       </c>
     </row>
-    <row r="124" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>122</v>
       </c>
@@ -58136,7 +58152,7 @@
         <v>0.21519195161613541</v>
       </c>
     </row>
-    <row r="125" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>123</v>
       </c>
@@ -58591,7 +58607,7 @@
         <v>0.37458907183263951</v>
       </c>
     </row>
-    <row r="126" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>124</v>
       </c>
@@ -59046,7 +59062,7 @@
         <v>0.22442694867576929</v>
       </c>
     </row>
-    <row r="127" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>125</v>
       </c>
@@ -59501,7 +59517,7 @@
         <v>0.24737190262273881</v>
       </c>
     </row>
-    <row r="128" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>126</v>
       </c>
@@ -59956,7 +59972,7 @@
         <v>0.246922855876406</v>
       </c>
     </row>
-    <row r="129" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>127</v>
       </c>
@@ -60411,7 +60427,7 @@
         <v>0.28036087463640741</v>
       </c>
     </row>
-    <row r="130" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>128</v>
       </c>
@@ -60866,7 +60882,7 @@
         <v>0.2506051536276066</v>
       </c>
     </row>
-    <row r="131" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>129</v>
       </c>
@@ -61321,7 +61337,7 @@
         <v>0.1979033190009778</v>
       </c>
     </row>
-    <row r="132" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>130</v>
       </c>
@@ -61776,7 +61792,7 @@
         <v>0.21705364280627501</v>
       </c>
     </row>
-    <row r="133" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>131</v>
       </c>
@@ -62231,7 +62247,7 @@
         <v>0.1863494771528407</v>
       </c>
     </row>
-    <row r="134" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>132</v>
       </c>
@@ -62686,7 +62702,7 @@
         <v>0.246922855876406</v>
       </c>
     </row>
-    <row r="135" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>133</v>
       </c>
@@ -63141,7 +63157,7 @@
         <v>0.15575506116940779</v>
       </c>
     </row>
-    <row r="136" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>134</v>
       </c>
@@ -63596,7 +63612,7 @@
         <v>0.1066466452487376</v>
       </c>
     </row>
-    <row r="137" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>135</v>
       </c>
@@ -64051,7 +64067,7 @@
         <v>0.11084703306078419</v>
       </c>
     </row>
-    <row r="138" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>136</v>
       </c>
@@ -64506,7 +64522,7 @@
         <v>0.1248576350595634</v>
       </c>
     </row>
-    <row r="139" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>137</v>
       </c>
@@ -64961,7 +64977,7 @@
         <v>6.0802028592363819E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>138</v>
       </c>
@@ -65416,7 +65432,7 @@
         <v>5.2174363828767001E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>139</v>
       </c>
@@ -65871,7 +65887,7 @@
         <v>0.12022796462994489</v>
       </c>
     </row>
-    <row r="142" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>140</v>
       </c>
@@ -66326,7 +66342,7 @@
         <v>0.1339436197051323</v>
       </c>
     </row>
-    <row r="143" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>141</v>
       </c>
@@ -66781,7 +66797,7 @@
         <v>0.16212559759049369</v>
       </c>
     </row>
-    <row r="144" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>142</v>
       </c>
@@ -67236,7 +67252,7 @@
         <v>9.8400150181543355E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>143</v>
       </c>
@@ -67691,7 +67707,7 @@
         <v>0.14112967145727201</v>
       </c>
     </row>
-    <row r="146" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>144</v>
       </c>
@@ -68146,7 +68162,7 @@
         <v>0.25969117977764872</v>
       </c>
     </row>
-    <row r="147" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>145</v>
       </c>
@@ -68601,7 +68617,7 @@
         <v>0.13864036219705239</v>
       </c>
     </row>
-    <row r="148" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>146</v>
       </c>
@@ -69056,7 +69072,7 @@
         <v>0.19896391374266281</v>
       </c>
     </row>
-    <row r="149" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>147</v>
       </c>
@@ -69511,7 +69527,7 @@
         <v>9.258586145773294E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>148</v>
       </c>
@@ -69966,7 +69982,7 @@
         <v>9.258586145773294E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:151" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:151" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>149</v>
       </c>
@@ -70419,6 +70435,1682 @@
       </c>
       <c r="EU151">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B33640B-10E7-4382-A73A-D01F38895C41}">
+  <dimension ref="A1:C151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C151"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>121.527697</v>
+      </c>
+      <c r="C2" s="2">
+        <v>25.020610000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>121.534509</v>
+      </c>
+      <c r="C3" s="2">
+        <v>25.014289000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>121.530556</v>
+      </c>
+      <c r="C4" s="2">
+        <v>25.017032</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>121.530169</v>
+      </c>
+      <c r="C5" s="2">
+        <v>25.017150999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>121.53142</v>
+      </c>
+      <c r="C6" s="2">
+        <v>25.016172999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>121.529689</v>
+      </c>
+      <c r="C7" s="2">
+        <v>25.018920000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>121.531904</v>
+      </c>
+      <c r="C8" s="2">
+        <v>25.01681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>121.529537</v>
+      </c>
+      <c r="C9" s="2">
+        <v>25.019120000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>121.532366</v>
+      </c>
+      <c r="C10" s="2">
+        <v>25.015775000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>121.52810700000001</v>
+      </c>
+      <c r="C11" s="2">
+        <v>25.018276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>121.52828100000001</v>
+      </c>
+      <c r="C12" s="2">
+        <v>25.017963000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>121.533115</v>
+      </c>
+      <c r="C13" s="2">
+        <v>25.015640000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>121.531109</v>
+      </c>
+      <c r="C14" s="2">
+        <v>25.016528999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>121.531254</v>
+      </c>
+      <c r="C15" s="2">
+        <v>25.016779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>121.530216</v>
+      </c>
+      <c r="C16" s="2">
+        <v>25.017806</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>121.534274</v>
+      </c>
+      <c r="C17" s="2">
+        <v>25.014503000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>121.533978</v>
+      </c>
+      <c r="C18" s="2">
+        <v>25.014786000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>121.534572</v>
+      </c>
+      <c r="C19" s="2">
+        <v>25.014230000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>121.534244</v>
+      </c>
+      <c r="C20" s="2">
+        <v>25.013397000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <v>121.53628399999999</v>
+      </c>
+      <c r="C21" s="2">
+        <v>25.012540000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <v>121.53501</v>
+      </c>
+      <c r="C22" s="2">
+        <v>25.013760000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>121.53501</v>
+      </c>
+      <c r="C23" s="2">
+        <v>25.013760000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <v>121.536641</v>
+      </c>
+      <c r="C24" s="2">
+        <v>25.011340000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
+        <v>121.530593</v>
+      </c>
+      <c r="C25" s="2">
+        <v>25.013590000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
+        <v>121.534381</v>
+      </c>
+      <c r="C26" s="2">
+        <v>25.013380000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <v>121.533675</v>
+      </c>
+      <c r="C27" s="2">
+        <v>25.013282</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2">
+        <v>121.52699</v>
+      </c>
+      <c r="C28" s="2">
+        <v>25.019131000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2">
+        <v>121.528239</v>
+      </c>
+      <c r="C29" s="2">
+        <v>25.019309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
+        <v>121.527218</v>
+      </c>
+      <c r="C30" s="2">
+        <v>25.020164000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2">
+        <v>121.527889</v>
+      </c>
+      <c r="C31" s="2">
+        <v>25.020046000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2">
+        <v>121.526651</v>
+      </c>
+      <c r="C32" s="2">
+        <v>25.020700000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <v>121.527416</v>
+      </c>
+      <c r="C33" s="2">
+        <v>25.020109000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2">
+        <v>121.527535</v>
+      </c>
+      <c r="C34" s="2">
+        <v>25.020052</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2">
+        <v>121.52342400000001</v>
+      </c>
+      <c r="C35" s="2">
+        <v>25.019507000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2">
+        <v>121.528153</v>
+      </c>
+      <c r="C36" s="2">
+        <v>25.020439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2">
+        <v>121.528694</v>
+      </c>
+      <c r="C37" s="2">
+        <v>25.019952</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2">
+        <v>121.523853</v>
+      </c>
+      <c r="C38" s="2">
+        <v>25.018757999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2">
+        <v>121.526619</v>
+      </c>
+      <c r="C39" s="2">
+        <v>25.019669</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2">
+        <v>121.526473</v>
+      </c>
+      <c r="C40" s="2">
+        <v>25.019062000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2">
+        <v>121.525448</v>
+      </c>
+      <c r="C41" s="2">
+        <v>25.020202000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2">
+        <v>121.527868</v>
+      </c>
+      <c r="C42" s="2">
+        <v>25.019321000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2">
+        <v>121.531279</v>
+      </c>
+      <c r="C43" s="2">
+        <v>25.015322000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2">
+        <v>121.530574</v>
+      </c>
+      <c r="C44" s="2">
+        <v>25.014308</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2">
+        <v>121.53151800000001</v>
+      </c>
+      <c r="C45" s="2">
+        <v>25.015464000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2">
+        <v>121.531734</v>
+      </c>
+      <c r="C46" s="2">
+        <v>25.015339000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2">
+        <v>121.531049</v>
+      </c>
+      <c r="C47" s="2">
+        <v>25.015647000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2">
+        <v>121.530835</v>
+      </c>
+      <c r="C48" s="2">
+        <v>25.015412000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2">
+        <v>121.531583</v>
+      </c>
+      <c r="C49" s="2">
+        <v>25.014735000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2">
+        <v>121.530322</v>
+      </c>
+      <c r="C50" s="2">
+        <v>25.015549</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2">
+        <v>121.52938</v>
+      </c>
+      <c r="C51" s="2">
+        <v>25.013065000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2">
+        <v>121.530175</v>
+      </c>
+      <c r="C52" s="2">
+        <v>25.020029000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2">
+        <v>121.529895</v>
+      </c>
+      <c r="C53" s="2">
+        <v>25.019379000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2">
+        <v>121.530658</v>
+      </c>
+      <c r="C54" s="2">
+        <v>25.019120999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2">
+        <v>121.530141</v>
+      </c>
+      <c r="C55" s="2">
+        <v>25.019143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2">
+        <v>121.53031</v>
+      </c>
+      <c r="C56" s="2">
+        <v>25.019479</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2">
+        <v>121.529976</v>
+      </c>
+      <c r="C57" s="2">
+        <v>25.019303000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2">
+        <v>121.529946</v>
+      </c>
+      <c r="C58" s="2">
+        <v>25.019825000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2">
+        <v>121.529803</v>
+      </c>
+      <c r="C59" s="2">
+        <v>25.019466000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2">
+        <v>121.53028</v>
+      </c>
+      <c r="C60" s="2">
+        <v>25.019523</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2">
+        <v>121.530523</v>
+      </c>
+      <c r="C61" s="2">
+        <v>25.019241000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2">
+        <v>121.53039</v>
+      </c>
+      <c r="C62" s="2">
+        <v>25.019348000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2">
+        <v>121.530421</v>
+      </c>
+      <c r="C63" s="2">
+        <v>25.019853000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2">
+        <v>121.530368</v>
+      </c>
+      <c r="C64" s="2">
+        <v>25.018903000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2">
+        <v>121.530703</v>
+      </c>
+      <c r="C65" s="2">
+        <v>25.018587</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2">
+        <v>121.53074700000001</v>
+      </c>
+      <c r="C66" s="2">
+        <v>25.018543000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2">
+        <v>121.53074700000001</v>
+      </c>
+      <c r="C67" s="2">
+        <v>25.018543000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2">
+        <v>121.53133</v>
+      </c>
+      <c r="C68" s="2">
+        <v>25.017969999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="2">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2">
+        <v>121.530884</v>
+      </c>
+      <c r="C69" s="2">
+        <v>25.018894</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2">
+        <v>121.531465</v>
+      </c>
+      <c r="C70" s="2">
+        <v>25.019293000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2">
+        <v>121.530575</v>
+      </c>
+      <c r="C71" s="2">
+        <v>25.019411000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2">
+        <v>121.531662</v>
+      </c>
+      <c r="C72" s="2">
+        <v>25.019852</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="2">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2">
+        <v>121.531026</v>
+      </c>
+      <c r="C73" s="2">
+        <v>25.019621999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="2">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2">
+        <v>121.53077500000001</v>
+      </c>
+      <c r="C74" s="2">
+        <v>25.019821</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="2">
+        <v>73</v>
+      </c>
+      <c r="B75" s="2">
+        <v>121.531431</v>
+      </c>
+      <c r="C75" s="2">
+        <v>25.019462999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="2">
+        <v>74</v>
+      </c>
+      <c r="B76" s="2">
+        <v>121.531268</v>
+      </c>
+      <c r="C76" s="2">
+        <v>25.018621</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="2">
+        <v>75</v>
+      </c>
+      <c r="B77" s="2">
+        <v>121.530956</v>
+      </c>
+      <c r="C77" s="2">
+        <v>25.018343000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="2">
+        <v>76</v>
+      </c>
+      <c r="B78" s="2">
+        <v>121.530956</v>
+      </c>
+      <c r="C78" s="2">
+        <v>25.018343000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="2">
+        <v>77</v>
+      </c>
+      <c r="B79" s="2">
+        <v>121.532386</v>
+      </c>
+      <c r="C79" s="2">
+        <v>25.021117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="2">
+        <v>78</v>
+      </c>
+      <c r="B80" s="2">
+        <v>121.532918</v>
+      </c>
+      <c r="C80" s="2">
+        <v>25.020600000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="2">
+        <v>79</v>
+      </c>
+      <c r="B81" s="2">
+        <v>121.532152</v>
+      </c>
+      <c r="C81" s="2">
+        <v>25.020671</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="2">
+        <v>80</v>
+      </c>
+      <c r="B82" s="2">
+        <v>121.53249</v>
+      </c>
+      <c r="C82" s="2">
+        <v>25.020461000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="2">
+        <v>81</v>
+      </c>
+      <c r="B83" s="2">
+        <v>121.5324</v>
+      </c>
+      <c r="C83" s="2">
+        <v>25.020910000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="2">
+        <v>82</v>
+      </c>
+      <c r="B84" s="2">
+        <v>121.53234</v>
+      </c>
+      <c r="C84" s="2">
+        <v>25.021393</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="2">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2">
+        <v>121.532889</v>
+      </c>
+      <c r="C85" s="2">
+        <v>25.021360000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="2">
+        <v>84</v>
+      </c>
+      <c r="B86" s="2">
+        <v>121.53282900000001</v>
+      </c>
+      <c r="C86" s="2">
+        <v>25.021360000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="2">
+        <v>85</v>
+      </c>
+      <c r="B87" s="2">
+        <v>121.532854</v>
+      </c>
+      <c r="C87" s="2">
+        <v>25.020244000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="2">
+        <v>86</v>
+      </c>
+      <c r="B88" s="2">
+        <v>121.532957</v>
+      </c>
+      <c r="C88" s="2">
+        <v>25.021712000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="2">
+        <v>87</v>
+      </c>
+      <c r="B89" s="2">
+        <v>121.532573</v>
+      </c>
+      <c r="C89" s="2">
+        <v>25.021744000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="2">
+        <v>88</v>
+      </c>
+      <c r="B90" s="2">
+        <v>121.53227</v>
+      </c>
+      <c r="C90" s="2">
+        <v>25.020043000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="2">
+        <v>89</v>
+      </c>
+      <c r="B91" s="2">
+        <v>121.531139</v>
+      </c>
+      <c r="C91" s="2">
+        <v>25.020852000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="2">
+        <v>90</v>
+      </c>
+      <c r="B92" s="2">
+        <v>121.531801</v>
+      </c>
+      <c r="C92" s="2">
+        <v>25.021415000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="2">
+        <v>91</v>
+      </c>
+      <c r="B93" s="2">
+        <v>121.531116</v>
+      </c>
+      <c r="C93" s="2">
+        <v>25.020409000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="2">
+        <v>92</v>
+      </c>
+      <c r="B94" s="2">
+        <v>121.532538</v>
+      </c>
+      <c r="C94" s="2">
+        <v>25.017150000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="2">
+        <v>93</v>
+      </c>
+      <c r="B95" s="2">
+        <v>121.53258</v>
+      </c>
+      <c r="C95" s="2">
+        <v>25.017603000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="2">
+        <v>94</v>
+      </c>
+      <c r="B96" s="2">
+        <v>121.532657</v>
+      </c>
+      <c r="C96" s="2">
+        <v>25.018297</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="2">
+        <v>95</v>
+      </c>
+      <c r="B97" s="2">
+        <v>121.532236</v>
+      </c>
+      <c r="C97" s="2">
+        <v>25.017077</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="2">
+        <v>96</v>
+      </c>
+      <c r="B98" s="2">
+        <v>121.532826</v>
+      </c>
+      <c r="C98" s="2">
+        <v>25.018073000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="2">
+        <v>97</v>
+      </c>
+      <c r="B99" s="2">
+        <v>121.531953</v>
+      </c>
+      <c r="C99" s="2">
+        <v>25.018799000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="2">
+        <v>98</v>
+      </c>
+      <c r="B100" s="2">
+        <v>121.531453</v>
+      </c>
+      <c r="C100" s="2">
+        <v>25.017835000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="2">
+        <v>99</v>
+      </c>
+      <c r="B101" s="2">
+        <v>121.532546</v>
+      </c>
+      <c r="C101" s="2">
+        <v>25.017219999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="2">
+        <v>100</v>
+      </c>
+      <c r="B102" s="2">
+        <v>121.531847</v>
+      </c>
+      <c r="C102" s="2">
+        <v>25.018359</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="2">
+        <v>101</v>
+      </c>
+      <c r="B103" s="2">
+        <v>121.531859</v>
+      </c>
+      <c r="C103" s="2">
+        <v>25.017447000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="2">
+        <v>102</v>
+      </c>
+      <c r="B104" s="2">
+        <v>121.532234</v>
+      </c>
+      <c r="C104" s="2">
+        <v>25.018090000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="2">
+        <v>103</v>
+      </c>
+      <c r="B105" s="2">
+        <v>121.531671</v>
+      </c>
+      <c r="C105" s="2">
+        <v>25.017633</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="2">
+        <v>104</v>
+      </c>
+      <c r="B106" s="2">
+        <v>121.532044</v>
+      </c>
+      <c r="C106" s="2">
+        <v>25.017484</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="2">
+        <v>105</v>
+      </c>
+      <c r="B107" s="2">
+        <v>121.531597</v>
+      </c>
+      <c r="C107" s="2">
+        <v>25.017703999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" s="2">
+        <v>106</v>
+      </c>
+      <c r="B108" s="2">
+        <v>121.53179</v>
+      </c>
+      <c r="C108" s="2">
+        <v>25.017516000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="2">
+        <v>107</v>
+      </c>
+      <c r="B109" s="2">
+        <v>121.53195100000001</v>
+      </c>
+      <c r="C109" s="2">
+        <v>25.018338</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="2">
+        <v>108</v>
+      </c>
+      <c r="B110" s="2">
+        <v>121.532116</v>
+      </c>
+      <c r="C110" s="2">
+        <v>25.018782000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" s="2">
+        <v>109</v>
+      </c>
+      <c r="B111" s="2">
+        <v>121.531931</v>
+      </c>
+      <c r="C111" s="2">
+        <v>25.017372000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" s="2">
+        <v>110</v>
+      </c>
+      <c r="B112" s="2">
+        <v>121.532917</v>
+      </c>
+      <c r="C112" s="2">
+        <v>25.017354000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" s="2">
+        <v>111</v>
+      </c>
+      <c r="B113" s="2">
+        <v>121.53278400000001</v>
+      </c>
+      <c r="C113" s="2">
+        <v>25.016743000000002</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="2">
+        <v>112</v>
+      </c>
+      <c r="B114" s="2">
+        <v>121.532436</v>
+      </c>
+      <c r="C114" s="2">
+        <v>25.016881000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="2">
+        <v>113</v>
+      </c>
+      <c r="B115" s="2">
+        <v>121.532709</v>
+      </c>
+      <c r="C115" s="2">
+        <v>25.017225</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="2">
+        <v>114</v>
+      </c>
+      <c r="B116" s="2">
+        <v>121.53276</v>
+      </c>
+      <c r="C116" s="2">
+        <v>25.019359000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="2">
+        <v>115</v>
+      </c>
+      <c r="B117" s="2">
+        <v>121.533192</v>
+      </c>
+      <c r="C117" s="2">
+        <v>25.019193000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="2">
+        <v>116</v>
+      </c>
+      <c r="B118" s="2">
+        <v>121.5325</v>
+      </c>
+      <c r="C118" s="2">
+        <v>25.019555</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="2">
+        <v>117</v>
+      </c>
+      <c r="B119" s="2">
+        <v>121.532203</v>
+      </c>
+      <c r="C119" s="2">
+        <v>25.019438000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="2">
+        <v>118</v>
+      </c>
+      <c r="B120" s="2">
+        <v>121.532197</v>
+      </c>
+      <c r="C120" s="2">
+        <v>25.019221000000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="2">
+        <v>119</v>
+      </c>
+      <c r="B121" s="2">
+        <v>121.532174</v>
+      </c>
+      <c r="C121" s="2">
+        <v>25.019041000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="2">
+        <v>120</v>
+      </c>
+      <c r="B122" s="2">
+        <v>121.53193</v>
+      </c>
+      <c r="C122" s="2">
+        <v>25.019465</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="2">
+        <v>121</v>
+      </c>
+      <c r="B123" s="2">
+        <v>121.532867</v>
+      </c>
+      <c r="C123" s="2">
+        <v>25.017361000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="2">
+        <v>122</v>
+      </c>
+      <c r="B124" s="2">
+        <v>121.53278400000001</v>
+      </c>
+      <c r="C124" s="2">
+        <v>25.016743000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="2">
+        <v>123</v>
+      </c>
+      <c r="B125" s="2">
+        <v>121.533964</v>
+      </c>
+      <c r="C125" s="2">
+        <v>25.021920000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" s="2">
+        <v>124</v>
+      </c>
+      <c r="B126" s="2">
+        <v>121.53384800000001</v>
+      </c>
+      <c r="C126" s="2">
+        <v>25.020568999999998</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="2">
+        <v>125</v>
+      </c>
+      <c r="B127" s="2">
+        <v>121.533818</v>
+      </c>
+      <c r="C127" s="2">
+        <v>25.020783000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="2">
+        <v>126</v>
+      </c>
+      <c r="B128" s="2">
+        <v>121.5337</v>
+      </c>
+      <c r="C128" s="2">
+        <v>25.020793000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="2">
+        <v>127</v>
+      </c>
+      <c r="B129" s="2">
+        <v>121.533559</v>
+      </c>
+      <c r="C129" s="2">
+        <v>25.021104000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="2">
+        <v>128</v>
+      </c>
+      <c r="B130" s="2">
+        <v>121.533503</v>
+      </c>
+      <c r="C130" s="2">
+        <v>25.020838000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="2">
+        <v>129</v>
+      </c>
+      <c r="B131" s="2">
+        <v>121.53352700000001</v>
+      </c>
+      <c r="C131" s="2">
+        <v>25.020363</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="2">
+        <v>130</v>
+      </c>
+      <c r="B132" s="2">
+        <v>121.533446</v>
+      </c>
+      <c r="C132" s="2">
+        <v>25.020537000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="2">
+        <v>131</v>
+      </c>
+      <c r="B133" s="2">
+        <v>121.533033</v>
+      </c>
+      <c r="C133" s="2">
+        <v>25.020219999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="2">
+        <v>132</v>
+      </c>
+      <c r="B134" s="2">
+        <v>121.5337</v>
+      </c>
+      <c r="C134" s="2">
+        <v>25.020793000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="2">
+        <v>133</v>
+      </c>
+      <c r="B135" s="2">
+        <v>121.533362</v>
+      </c>
+      <c r="C135" s="2">
+        <v>25.019984000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="2">
+        <v>134</v>
+      </c>
+      <c r="B136" s="2">
+        <v>121.533424</v>
+      </c>
+      <c r="C136" s="2">
+        <v>25.019544</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="2">
+        <v>135</v>
+      </c>
+      <c r="B137" s="2">
+        <v>121.53319</v>
+      </c>
+      <c r="C137" s="2">
+        <v>25.019556000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="2">
+        <v>136</v>
+      </c>
+      <c r="B138" s="2">
+        <v>121.533225</v>
+      </c>
+      <c r="C138" s="2">
+        <v>25.019691000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="2">
+        <v>137</v>
+      </c>
+      <c r="B139" s="2">
+        <v>121.53339</v>
+      </c>
+      <c r="C139" s="2">
+        <v>25.019130000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="2">
+        <v>138</v>
+      </c>
+      <c r="B140" s="2">
+        <v>121.533355</v>
+      </c>
+      <c r="C140" s="2">
+        <v>25.018122000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="2">
+        <v>139</v>
+      </c>
+      <c r="B141" s="2">
+        <v>121.533233</v>
+      </c>
+      <c r="C141" s="2">
+        <v>25.017520000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="2">
+        <v>140</v>
+      </c>
+      <c r="B142" s="2">
+        <v>121.533</v>
+      </c>
+      <c r="C142" s="2">
+        <v>25.017448000000002</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="2">
+        <v>141</v>
+      </c>
+      <c r="B143" s="2">
+        <v>121.53300900000001</v>
+      </c>
+      <c r="C143" s="2">
+        <v>25.01999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="2">
+        <v>142</v>
+      </c>
+      <c r="B144" s="2">
+        <v>121.53295</v>
+      </c>
+      <c r="C144" s="2">
+        <v>25.019351</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="2">
+        <v>143</v>
+      </c>
+      <c r="B145" s="2">
+        <v>121.53323</v>
+      </c>
+      <c r="C145" s="2">
+        <v>25.019839999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="2">
+        <v>144</v>
+      </c>
+      <c r="B146" s="2">
+        <v>121.531363</v>
+      </c>
+      <c r="C146" s="2">
+        <v>25.019969</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" s="2">
+        <v>145</v>
+      </c>
+      <c r="B147" s="2">
+        <v>121.532729</v>
+      </c>
+      <c r="C147" s="2">
+        <v>25.017517000000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="2">
+        <v>146</v>
+      </c>
+      <c r="B148" s="2">
+        <v>121.533801</v>
+      </c>
+      <c r="C148" s="2">
+        <v>25.020344000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="2">
+        <v>147</v>
+      </c>
+      <c r="B149" s="2">
+        <v>121.533196</v>
+      </c>
+      <c r="C149" s="2">
+        <v>25.017782</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" s="2">
+        <v>148</v>
+      </c>
+      <c r="B150" s="2">
+        <v>121.533196</v>
+      </c>
+      <c r="C150" s="2">
+        <v>25.017782</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" s="2">
+        <v>149</v>
+      </c>
+      <c r="B151" s="2">
+        <v>121.533439</v>
+      </c>
+      <c r="C151" s="2">
+        <v>25.018585000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>